<commit_message>
Wijziging: uitwerking EDA  voorbeelden
</commit_message>
<xml_diff>
--- a/_book/data/vakanties.xlsx
+++ b/_book/data/vakanties.xlsx
@@ -1,64 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBC9CC1-617C-4F3B-A473-03F5E26025E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\studieboeken\excelanalyse\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBCB80B-0781-4573-B5A3-2FB51AEC5EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EAEBF272-D7AE-452D-AAF4-FD03D98EC6C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vakanties" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="10">
   <si>
-    <t>Leeftijdsklasse</t>
+    <t>id</t>
   </si>
   <si>
-    <t>Vakantieland</t>
+    <t>leeftijdsklasse</t>
+  </si>
+  <si>
+    <t>vakantieland</t>
+  </si>
+  <si>
+    <t>oud</t>
+  </si>
+  <si>
+    <t>Turkije</t>
   </si>
   <si>
     <t>middelbaar</t>
   </si>
   <si>
-    <t>Turkije</t>
-  </si>
-  <si>
-    <t>oud</t>
+    <t>Griekenland</t>
   </si>
   <si>
     <t>Spanje</t>
   </si>
   <si>
-    <t>Griekenland</t>
-  </si>
-  <si>
-    <t>Italië</t>
-  </si>
-  <si>
     <t>jong</t>
   </si>
   <si>
-    <t>id</t>
+    <t>Italie</t>
   </si>
 </sst>
 </file>
@@ -68,7 +59,7 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,8 +104,20 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TabelVakanties" displayName="TabelVakanties" ref="A1:C201" totalsRowShown="0">
+  <autoFilter ref="A1:C201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="leeftijdsklasse"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="vakantieland"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -124,45 +127,41 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -189,32 +188,11 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -241,23 +219,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -269,169 +230,193 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83B4AAD-C165-4C95-913E-89F8C42AE7E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,10 +424,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,10 +435,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,10 +446,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -483,10 +468,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,10 +479,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -505,10 +490,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,10 +501,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,10 +512,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,10 +523,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -560,10 +545,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,7 +556,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -582,10 +567,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -593,10 +578,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,10 +589,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -615,10 +600,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,10 +611,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,10 +622,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,10 +633,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,10 +644,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -670,10 +655,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,10 +666,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -692,10 +677,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,7 +688,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -714,10 +699,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,10 +710,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,10 +721,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -747,10 +732,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,10 +743,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,10 +754,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,10 +765,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,10 +776,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,10 +787,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -813,10 +798,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,10 +809,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,7 +820,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -846,7 +831,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -857,10 +842,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,10 +853,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,7 +864,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -890,10 +875,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,10 +886,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,10 +897,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,10 +908,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,10 +919,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,10 +930,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,10 +941,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,10 +952,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -978,10 +963,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,7 +974,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -1000,7 +985,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -1011,10 +996,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,10 +1007,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1033,10 +1018,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1029,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
@@ -1055,10 +1040,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,7 +1051,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
@@ -1077,10 +1062,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,10 +1073,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,10 +1084,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,10 +1095,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,10 +1106,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1132,7 +1117,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
@@ -1143,10 +1128,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,10 +1139,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,10 +1150,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,7 +1161,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
@@ -1187,10 +1172,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,10 +1183,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,10 +1194,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,10 +1205,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,10 +1216,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1242,10 +1227,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,7 +1238,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -1264,10 +1249,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,10 +1271,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1297,10 +1282,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,10 +1293,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1319,10 +1304,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,10 +1315,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1341,10 +1326,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1352,10 +1337,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1363,10 +1348,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,10 +1359,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1385,10 +1370,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1396,10 +1381,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1407,7 +1392,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
@@ -1418,10 +1403,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,10 +1414,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1440,10 +1425,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1451,10 +1436,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1462,10 +1447,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1473,7 +1458,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
@@ -1484,10 +1469,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,10 +1480,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1506,10 +1491,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1517,10 +1502,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,7 +1513,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C101" t="s">
         <v>6</v>
@@ -1539,10 +1524,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,7 +1535,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C103" t="s">
         <v>7</v>
@@ -1561,10 +1546,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1572,10 +1557,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1586,7 +1571,7 @@
         <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1594,7 +1579,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C107" t="s">
         <v>7</v>
@@ -1605,10 +1590,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1616,10 +1601,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,10 +1612,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C110" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1638,10 +1623,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,7 +1634,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
         <v>6</v>
@@ -1660,10 +1645,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,10 +1656,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1682,10 +1667,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1693,10 +1678,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,10 +1689,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1715,7 +1700,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
@@ -1726,10 +1711,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C119" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -1737,10 +1722,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,10 +1733,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,7 +1744,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C122" t="s">
         <v>6</v>
@@ -1770,10 +1755,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1781,10 +1766,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1792,10 +1777,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1803,10 +1788,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C126" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -1814,10 +1799,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,7 +1813,7 @@
         <v>8</v>
       </c>
       <c r="C128" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -1836,10 +1821,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -1847,10 +1832,10 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -1858,10 +1843,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -1869,10 +1854,10 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C132" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -1880,10 +1865,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C133" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -1891,10 +1876,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C134" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1902,10 +1887,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C135" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,10 +1898,10 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -1924,10 +1909,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -1935,10 +1920,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -1946,10 +1931,10 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -1957,10 +1942,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -1968,10 +1953,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C141" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -1979,10 +1964,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C142" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,10 +1975,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2001,10 +1986,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C144" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2012,7 +1997,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C145" t="s">
         <v>6</v>
@@ -2023,10 +2008,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2034,10 +2019,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C147" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2045,7 +2030,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C148" t="s">
         <v>6</v>
@@ -2056,7 +2041,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C149" t="s">
         <v>6</v>
@@ -2067,7 +2052,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C150" t="s">
         <v>6</v>
@@ -2078,10 +2063,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C151" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2089,10 +2074,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2100,10 +2085,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2111,10 +2096,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C154" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2122,10 +2107,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2121,7 @@
         <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2144,10 +2129,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C157" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2155,10 +2140,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2166,10 +2151,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2177,10 +2162,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C160" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2188,10 +2173,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2199,10 +2184,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C162" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2210,10 +2195,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C163" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2221,10 +2206,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2232,10 +2217,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C165" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2243,10 +2228,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C166" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2254,10 +2239,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,10 +2250,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2276,10 +2261,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,10 +2272,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2298,10 +2283,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2309,10 +2294,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C172" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,10 +2305,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2331,10 +2316,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2342,10 +2327,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C175" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2353,7 +2338,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C176" t="s">
         <v>6</v>
@@ -2364,10 +2349,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C177" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2375,10 +2360,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C178" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2386,7 +2371,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C179" t="s">
         <v>6</v>
@@ -2397,10 +2382,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C180" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2408,10 +2393,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C181" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2419,10 +2404,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C182" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2430,10 +2415,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C183" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2441,10 +2426,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C184" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2452,10 +2437,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C185" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2463,7 +2448,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C186" t="s">
         <v>6</v>
@@ -2474,10 +2459,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -2485,10 +2470,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -2496,10 +2481,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C189" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -2510,7 +2495,7 @@
         <v>8</v>
       </c>
       <c r="C190" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2518,10 +2503,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C191" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2529,7 +2514,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C192" t="s">
         <v>6</v>
@@ -2540,10 +2525,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C193" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -2551,10 +2536,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C194" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2562,10 +2547,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C195" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2573,10 +2558,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C196" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2584,7 +2569,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C197" t="s">
         <v>6</v>
@@ -2595,7 +2580,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C198" t="s">
         <v>6</v>
@@ -2606,10 +2591,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C199" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2617,10 +2602,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C200" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2628,7 +2613,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C201" t="s">
         <v>6</v>
@@ -2636,6 +2621,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>